<commit_message>
feat/affixes tool (to be tested)
</commit_message>
<xml_diff>
--- a/querySparql.xlsx
+++ b/querySparql.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzofilitti/Desktop/SparqlAgent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20061274-E488-2343-9A3A-EE4056DB046D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275A9250-36B5-744B-A689-D13F7E8110BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16700" xr2:uid="{7EA1D7AC-A08B-ED4C-963B-D0B97934D44B}"/>
+    <workbookView xWindow="20" yWindow="780" windowWidth="29400" windowHeight="16700" xr2:uid="{7EA1D7AC-A08B-ED4C-963B-D0B97934D44B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="179">
   <si>
     <t>question</t>
   </si>
@@ -1631,6 +1631,17 @@
 	?resource a lime:Lexicon;
   			dcterms:title ?title
 }</t>
+  </si>
+  <si>
+    <t>select ?lemma ?label ?prefix where {
+  ?lemma a lila:Lemma;
+    	lila:hasPrefix prefix:5;
+  		rdfs:label ?label.
+  prefix:5 rdfs:label ?prefix
+}limit 1</t>
+  </si>
+  <si>
+    <t>Show me an example of a lemma starting with the prefix "ad"</t>
   </si>
 </sst>
 </file>
@@ -2011,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1300A24D-80E3-9B4F-82C4-C9F4C7D1290C}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2743,6 +2754,14 @@
         <v>176</v>
       </c>
     </row>
+    <row r="91" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new search similarity, improved response pipeline, reordered files
</commit_message>
<xml_diff>
--- a/querySparql.xlsx
+++ b/querySparql.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzofilitti/Desktop/SparqlAgent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275A9250-36B5-744B-A689-D13F7E8110BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A00545-EBA5-E045-A401-43980255FDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="780" windowWidth="29400" windowHeight="16700" xr2:uid="{7EA1D7AC-A08B-ED4C-963B-D0B97934D44B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19520" xr2:uid="{7EA1D7AC-A08B-ED4C-963B-D0B97934D44B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="192">
   <si>
     <t>question</t>
   </si>
@@ -95,9 +95,6 @@
     	lila:hasPOS ?pos;
 		lila:hasInflectionType lila:n6i.
 }limit 20</t>
-  </si>
-  <si>
-    <t>lila adjectivs that end in -ius</t>
   </si>
   <si>
     <t xml:space="preserve">first class pronominal adjective with dative singular ending in -i </t>
@@ -773,69 +770,6 @@
     <t>Retrieve all the lemmas with a Greek etymology (and thus included in the "Index Graecorum Vocabulorum in Linguam Latinam")</t>
   </si>
   <si>
-    <t>SELECT distinct ?tokenNoun ?tokenAdjLabel ?tokenNounLabel  ?tokenVerbLabel  ?wordnetSys
-WHERE {
-  VALUES ?corpora {
-    &lt;http://lila-erc.eu/data/corpora/ITTB/id/corpus&gt; 
-  }
-  VALUES ?synFunctionsUD {
-    UDSynFunction:obj
-  }
-  VALUES ?pos {
-    &lt;http://lila-erc.eu/ontologies/lila/proper_noun&gt; &lt;http://lila-erc.eu/ontologies/lila/noun&gt;
-  }
-  VALUES ?synFunctionsPDT {
-    ITTBSynFunction:Obj
-  }
-  VALUES ?wordnetSys {
-    &lt;http://lila-erc.eu/data/lexicalResources/LatinWordNet/id/LexicalConcept/01093838-v&gt; &lt;http://lila-erc.eu/data/lexicalResources/LatinWordNet/id/LexicalConcept/00866139-v&gt;
-  }
-  VALUES ?liber {
-  &lt;http://lila-erc.eu/data/corpora/ITTB/id/citationUnit/005.LB4.&gt;
-  }
-  ?corpora powla:hasSubDocument ?doc.
-  ?citLayer powla:hasDocument ?doc.
-  ?citLayer lilaCorpora:isLayer ?liber.
-  ?liber lilaCorpora:hasCitSubUnit*/powla:hasChild ?tokenNoun. 
-  ?tokenNoun powla:hasLayer/powla:hasDocument ?doc.
-  ?tokenNoun rdf:type powla:Terminal;
-             lila:hasLemma ?lemmaNoun ;
-             powla:hasStringValue ?tokenNounLabel.
-  ?lemmaNoun lila:hasPOS ?pos ;
-             rdfs:label ?lemmaNounLabel.
-  ?tokenVerb lila:hasLemma ?lemmaVerb ;
-             powla:hasStringValue ?tokenVerbLabel.
-  ?lemmaVerb lila:hasPOS &lt;http://lila-erc.eu/ontologies/lila/verb&gt; ;
-             rdfs:label ?lemmaVerbLabel.
-  &lt;http://lila-erc.eu/data/lexicalResources/LatinWordNet/Lexicon&gt; lime:entry ?leWordnet.
-  ?leWordnet ontolex:canonicalForm ?lemmaVerb;
-             ontolex:evokes ?wordnetSys.
-  ?rel rdf:type ?synFunctionsPDT ,lilacorpora:DependencyRel ;
-       lilacorpora:hasHead ?tokenVerb ;
-       lilacorpora:hasDep ?tokenNoun .
-  minus{
-    ?rel2 rdf:type ?synFunctionsUD ,lilacorpora:DependencyRel ;
-          lilacorpora:hasHead ?tokenVerb ;
-          lilacorpora:hasDep ?tokenNoun .
-  }
-  ?relAdj rdf:type lilacorpora:DependencyRel ;
-          lilacorpora:hasHead ?tokenNoun ;
-          lilacorpora:hasDep ?adjToken .
-  ?adjToken rdf:type powla:Terminal;
-            lila:hasLemma ?lemmaAdj;
-            powla:hasStringValue ?tokenAdjLabel.
-  ?lemmaAdj lila:hasPOS &lt;http://lila-erc.eu/ontologies/lila/adjective&gt;;
-            rdfs:label ?lemmaAdjLabel.
-  &lt;http://lila-erc.eu/data/lexicalResources/LatinAffectus/Lexicon&gt; lime:entry ?leLemmaAdj.
-  ?leLemmaAdj ontolex:canonicalForm ?lemmaAdj;
-              ontolex:sense ?latinAffectusSense.
-  ?latinAffectusSense marl:hasPolarity marl:Positive.
-}</t>
-  </si>
-  <si>
-    <t>Chains in the ITTB where a common or proper noun depends as Obj in the PDT formalism and as obj in the UD formalism, on a verb belonging to either synset of "cause to seem less serious; play down" or "fight against or resist strongly", and is head of an adjective (in the LemmaBank) with positive polarity.</t>
-  </si>
-  <si>
     <t>SELECT (GROUP_CONCAT(DISTINCT ?wr ;
     separator=", ") as ?wrs) ?lemma ?freq 
 WHERE {
@@ -1153,28 +1087,6 @@
   </si>
   <si>
     <t>counts the number of distinct lemmas in LASLA for each inflection micro-class of verbs of the third conjugation.</t>
-  </si>
-  <si>
-    <t>SELECT ?formLabel  ?lemmaTargetLabel  ?form ?lemmaTarget  WHERE {
-  VALUES ?lemma {&lt;http://lila-erc.eu/data/id/lemma/118414&gt; }
-  VALUES ?cells {&lt;http://lila-erc.eu/data/lexicalResources/prinparlat/id/cell_prf.act.ind.1.sg&gt;  &lt;http://lila-erc.eu/data/lexicalResources/prinparlat/id/cell_prf.act.ind.3.sg&gt;  }
-  &lt;http://lila-erc.eu/data/lexicalResources/WFL/Lexicon&gt; lime:entry ?le.
-  ?le ontolex:canonicalForm ?lemma.
-  ?rule rdf:type &lt;http://lila-erc.eu/ontologies/lila/wfl/Prefixation/VerbToVerb&gt;.
-  ?rel &lt;http://www.w3.org/ns/lemon/vartrans#source&gt; ?le;
-       &lt;http://lila-erc.eu/ontologies/lila/wfl/hasWordFormationRule&gt; ?rule;
-       &lt;http://www.w3.org/ns/lemon/vartrans#target&gt; ?target .
-  ?target ontolex:canonicalForm ?lemmaTarget.
-  ?lemmaTarget rdfs:label ?lemmaTargetLabel.
-  ?flexeme ontolex:canonicalForm ?lemmaTarget.
-  ?form &lt;http://lila-erc.eu/ontologies/prinparlat/flexeme&gt; ?flexeme;
-        &lt;https://www.paralex-standard.org/paralex_ontology.xml#cell&gt; ?cells;
-        rdfs:label ?formLabel
-} group by ?form ?formLabel ?lemmaTarget ?lemmaTargetLabel 
-order by ?lemmaTargetLabel</t>
-  </si>
-  <si>
-    <t>extract all the perfect forms of all verbs that are directly derived from "pono" via prefixation according to WFL</t>
   </si>
   <si>
     <t>SELECT  ?lemma ?lemmaLabel WHERE {
@@ -1290,41 +1202,6 @@
     <t>Retrieves all lemmas whose entries in Lexicon Bohemorum include the word "natura" in their definition and do not occur also in the Lewis &amp; Short dictionary, and then returns the number of their occurrences in the textual corpora linked to LiLa.</t>
   </si>
   <si>
-    <t>SELECT  ?ep ?par (SUM(?v) as ?sentVal) (COUNT(?v) as ?count) 
-((SUM(?v) / COUNT(?v)) as ?normVal)
-WHERE {
-   ?CitationLayer powla:hasDocument 
-   &lt;http://lila-erc.eu/data/corpora/UDante/id/corpus/Epistole&gt;;
-                   lila_corpora:isLayer ?ep .
-  ?ep lila_corpora:hasCitSubUnit ?par .
-  ?par powla:hasChild ?token.
-  ?token lila:hasLemma ?lemma .   
-    VALUES ?polarity { marl:Positive marl:Negative } 
-        ?le ontolex:canonicalForm ?lemma ;
-        ontolex:sense ?sense .
-    ?sense marl:hasPolarity ?polarity ;
-       marl:polarityValue  ?v .
-} group by  ?ep ?par
-order by ?ep ?par</t>
-  </si>
-  <si>
-    <t>SELECT  ?ep (SUM(?v) as ?sentVal) (COUNT(?v) as ?count) 
-((SUM(?v) / COUNT(?v)) as ?normVal)
-WHERE {
-    VALUES ?polarity { marl:Positive marl:Negative } 
-        ?le ontolex:canonicalForm ?lemma ;
-        ontolex:sense ?sense .
-    ?sense marl:hasPolarity ?polarity ;
-          marl:polarityValue  ?v .
-    ?token lila:hasLemma ?lemma ;           
-      ^powla:hasChild/^lila_corpora:hasCitSubUnit ?ep.
-   ?CitationLayer powla:hasDocument 
-      &lt;http://lila-erc.eu/data/corpora/UDante/id/corpus/Epistole&gt;;
-                   lila_corpora:isLayer ?ep .
-} group by  (?ep)
-order by ?ep</t>
-  </si>
-  <si>
     <t>SELECT ?form (count(?form) as ?count) ?docTitle ?prefixlabel
 WHERE {
   ?le ontolex:canonicalForm ?lemma ;
@@ -1370,9 +1247,6 @@
 }</t>
   </si>
   <si>
-    <t>No question</t>
-  </si>
-  <si>
     <t>select ?doc ?title where{
   ?doc a powla:Document;
     	 dc:title ?title;
@@ -1642,6 +1516,84 @@
   </si>
   <si>
     <t>Show me an example of a lemma starting with the prefix "ad"</t>
+  </si>
+  <si>
+    <t>words with lemmas that start with the suffix "in"</t>
+  </si>
+  <si>
+    <t>SELECT ?lemmaLabel ?suffix ?lemma where{
+  	?lemma a lila:Lemma ;
+  			rdfs:label ?lemmaLabel;
+			lila:hasSuffix suffix:1.
+  	suffix:1 rdfs:label ?suffix
+}limit 10</t>
+  </si>
+  <si>
+    <t>What are the titles of the documents in the Lila knowledge base?</t>
+  </si>
+  <si>
+    <t>SELECT ?title WHERE {
+  ?doc a powla:Document ;
+       dc:title ?title .
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I'd like to see the first 5 documents and their titles.</t>
+  </si>
+  <si>
+    <t>SELECT ?resourceName WHERE {
+  ?resource a powla:Document ;
+            dc:title ?resourceName .
+}
+ORDER BY ?resourceName LIMIT 5</t>
+  </si>
+  <si>
+    <t>Can you display some documents with their titles from the database?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT ?docItem ?itemTitle WHERE {
+  ?docItem a powla:Document ;
+           dc:title ?itemTitle .
+} </t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>affix</t>
+  </si>
+  <si>
+    <t>lexical_resource</t>
+  </si>
+  <si>
+    <t>adjective</t>
+  </si>
+  <si>
+    <t>noun</t>
+  </si>
+  <si>
+    <t>lila adjectives that end in -ius</t>
+  </si>
+  <si>
+    <t>lemma</t>
+  </si>
+  <si>
+    <t>verb</t>
+  </si>
+  <si>
+    <t>corpus</t>
+  </si>
+  <si>
+    <t>etymology</t>
+  </si>
+  <si>
+    <t>inflection</t>
+  </si>
+  <si>
+    <t>synset</t>
   </si>
 </sst>
 </file>
@@ -2022,744 +1974,1018 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1300A24D-80E3-9B4F-82C4-C9F4C7D1290C}">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" customWidth="1"/>
-    <col min="2" max="2" width="136.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="136.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="272" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="272" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="17" spans="1:3" ht="272" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="272" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="204" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="204" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="238" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="21" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="306" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="306" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="238" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="255" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="221" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="221" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="388" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="388" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="30" spans="1:3" ht="204" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="221" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>188</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="289" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>190</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>186</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="388" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="187" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="204" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="238" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="221" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="153" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="255" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="289" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="238" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="388" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" s="1" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="255" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="43" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>186</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="289" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>186</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="289" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="221" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="1" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="221" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="49" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>191</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    </row>
+    <row r="50" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>191</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    </row>
+    <row r="52" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>186</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    </row>
+    <row r="53" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>186</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    </row>
+    <row r="54" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>186</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    </row>
+    <row r="55" spans="1:3" ht="289" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>186</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="255" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    </row>
+    <row r="56" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="289" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    </row>
+    <row r="57" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="187" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    </row>
+    <row r="58" spans="1:3" ht="356" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="238" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    </row>
+    <row r="59" spans="1:3" ht="289" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>186</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="356" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    </row>
+    <row r="60" spans="1:3" ht="323" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="340" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    </row>
+    <row r="61" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="289" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    </row>
+    <row r="62" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>186</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="323" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    </row>
+    <row r="63" spans="1:3" ht="289" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    </row>
+    <row r="64" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    </row>
+    <row r="65" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>180</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="306" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+    </row>
+    <row r="66" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>180</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>180</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>180</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="289" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="289" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="187" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="C70" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>180</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    </row>
+    <row r="72" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>180</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>188</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+    </row>
+    <row r="80" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>188</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="C80" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+      <c r="C81" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>188</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="C82" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B79" s="3" t="s">
+      <c r="C83" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B81" s="3" t="s">
+      <c r="C84" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>188</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>188</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>188</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B82" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+    <row r="89" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>182</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="C89" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>181</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>